<commit_message>
Inseriti dati mancanti nel dataset delle nascite
</commit_message>
<xml_diff>
--- a/dataset_puliti/nascite_pulito.xlsx
+++ b/dataset_puliti/nascite_pulito.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>298.5</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>373.7</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>229.1</t>
         </is>
       </c>
     </row>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>818.5</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>289</t>
         </is>
       </c>
     </row>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1880</t>
         </is>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>677.2</t>
         </is>
       </c>
     </row>
@@ -2978,32 +2978,32 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>734.5</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>739.3</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>743.8</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>747.4</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>749.6</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>750.3</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3028,12 +3028,12 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>636</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>629.4</t>
         </is>
       </c>
     </row>
@@ -3090,7 +3090,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>2890</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>2760</t>
         </is>
       </c>
     </row>
@@ -3313,32 +3313,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>26600</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>26030</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>25740</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>24900</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>24830</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3363,12 +3363,12 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>23140</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>23110</t>
         </is>
       </c>
     </row>
@@ -3380,32 +3380,32 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>617.6</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>613.2</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>602.8</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>592.9</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>584.7</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>577.6</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3539,37 +3539,37 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1890</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1690</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1610</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1490</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1440</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1400</t>
         </is>
       </c>
     </row>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>..</t>
+          <t>1180</t>
         </is>
       </c>
     </row>

</xml_diff>